<commit_message>
filtering out other multi binders
</commit_message>
<xml_diff>
--- a/files/20240314_additional_13_rAb_sequences_to_trim.xlsx
+++ b/files/20240314_additional_13_rAb_sequences_to_trim.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catherinenicholas/Hesselberth Lab Dropbox/Catherine Nicholas/My Mac (Catherine’s MacBook Pro)/Desktop/Experiments/Mia Experiments/Hu scSeq/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wellskr/Documents/sshfs/Analysis/Mia_Smith/Catherine_Nicolas/full_antigen_pos_data/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CDEF60-C8C7-914D-A0C4-05EC82760861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4BAC36-A70E-3849-8EBD-3F43DB897454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15940" xr2:uid="{6BF3BB73-7169-9A42-8FC8-569BE5755118}"/>
+    <workbookView xWindow="39580" yWindow="1940" windowWidth="27240" windowHeight="15940" xr2:uid="{6BF3BB73-7169-9A42-8FC8-569BE5755118}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="131">
   <si>
     <t>clone_id</t>
   </si>
@@ -411,6 +411,24 @@
   </si>
   <si>
     <t>ATGAGCAAAACTGACAAGTCAAGGCAGGAAGATGTTGCCATCACAACTCATTGGGTTTCTGCTGCTCTGGGTTCCAGCCTCCAGGGGTGAAATTGTGTTGACTCAGTCTCCAGAGTTTCAGTCTGTGACTCCAAAGGAGAAAGTCACCATCACCTGCCGGGCCAGTCAGAGCATTGGTCGTAGTTTACACTGGTACCAGCAGAAACCAGATCAGTCTCCAAAGCTCCTCATCAAGTATGCTTCCCAGTCCTTCTCAGGGGTCCCCTCGAGGTTCAGTGGCAGTGGATCTGGGACAGATTTCACCCTCACCATCAATAGCCTGGAAGCTGAAGATGCTGCAACGTATTACTGTCATCAGAGTAGTGGTTTACCCTGGACGTTCGGCCAAGGGACCAAGGTGGAAATCAAACGAACTGTGGCTGCACCATCTGTCTTCATCTTCCCGCCATCTGATGAGCAGTTGAAATCTGGAACTGCCTCTGTTGTGTGCCTGCTGAATAACTTCTATCCCAGAGAGGCCAAAGTACAGTGGAAGGTGGATAACGC</t>
+  </si>
+  <si>
+    <t>IGHV4-34;IGLV3-10</t>
+  </si>
+  <si>
+    <t>GCGAGAGGGGTTAGATATGATAGTAGTGGATATTACCCCACCTAC</t>
+  </si>
+  <si>
+    <t>TTTCTTATATGGGGAGTGCTTTCTGAGAGTCATGGACCTCCTGCACAAGAACATGAAACACCTGTGGTTCTTCCTCCTCCTGGTGGCAGCTCCCAGATGGGTCCTGTCCCAGGTGCAGCTACAGCAGTGGGGCGCAGGACTGTTGAAGCCTTCGGAGACCCTGTCCCTCACCTGCGCTGTCTATGGTGGGTCCTTCAGTGATTACTTCTGCACCTGGATCCGCCAGCCCCCAGGGAAGGGGCTGGAGTGGATTGGGGAAATCAATCATAGTGGAAGCAGCAACTACAACCCGTCCCTCAAGAGTCGAGTCACCATGTCATTAGACACGTCCAAGAACCAGTTCTCCCTGAGGTTGAGCTCTGTGACCGCCGCGGACACGGCTGTGTATTACTGTGCGAGAGGGGTTAGATATGATAGTAGTGGATATTACCCCACCTACTGGGGCCAGGGAACGCTGGTCACCGTCTCCTCAGGGAGTGCATCCGCCCCAACCCTTTTCCCCCTCGTCTCCTGTGAGAATTCCCCGTCGGATACGAGCAGCGTG;GTGGGCTCAGGAGGCAGAGCTCTGGGAATCTCACCATGGCCTGGACCCCTCTCCTGCTCCCCCTCCTCACTTTCTGCACAGTCTCTGAGGCCTCCTATGAGCTGACACAGCCACCCTCGGTGTCAGTGTCCCCAGGACAAACGGCCAGGATCACCTGCTCTGGAGATGCATTGCCAAAAAAATATGCTTATTGGTACCAGCAGAAGTCGGGCCAGGCCCCTGTGCTGGTCATCTATGAGGACAGCAAACGACCCTCCGGGATCCCTGGGAGATTCTCGGGCTCCACCTCAGGGACAATGGCCACCTTGACTATCAGTGGGGCCCAGGTGGAGGATGAAGCTGACTACTACTGTTACTCAACAGACAGCAGTACTAATTATAGGGTGTTCGGCGGAGGGACCAAGCTGACCGTCCTAGGTCAGCCCAAGGCTGCCCCCTCGGTCACTCTGTTCCCACCCTCCTCTGAGGAGCTTCAAGCCAACAAGGCCACACTGGTGTGTCTCATAAGTGACTTCTACCCGGGAGCCGTGGCAGTGGCCTGGAAGGCAGATAGCAGCCCCGTCGAGGCGGGAGTGGAGACCACCACACCCTCCAAACAAAGCAACAACAAGTACGCGGCCAGCAGCTA</t>
+  </si>
+  <si>
+    <t>TTTCTTATATGGGGAGTGCTTTCTGAGAGTCATGGACCTCCTGCACAAGAACATGAAACACCTGTGGTTCTTCCTCCTCCTGGTGGCAGCTCCCAGATGGGTCCTGTCCCAGGTGCAGCTACAGCAGTGGGGCGCAGGACTGTTGAAGCCTTCGGAGACCCTGTCCCTCACCTGCGCTGTCTATGGTGGGTCCTTCAGTGATTACTTCTGCACCTGGATCCGCCAGCCCCCAGGGAAGGGGCTGGAGTGGATTGGGGAAATCAATCATAGTGGAAGCAGCAACTACAACCCGTCCCTCAAGAGTCGAGTCACCATGTCATTAGACACGTCCAAGAACCAGTTCTCCCTGAGGTTGAGCTCTGTGACCGCCGCGGACACGGCTGTGTATTACTGTGCGAGAGGGGTTAGATATGATAGTAGTGGATATTACCCCACCTACTGGGGCCAGGGAACGCTGGTCACCGTCTCCTCAGGGAGTGCATCCGCCCCAACCCTTTTCCCCCTCGTCTCCTGTGAGAATTCCCCGTCGGATACGAGCAGCGTG</t>
+  </si>
+  <si>
+    <t>GTGGGCTCAGGAGGCAGAGCTCTGGGAATCTCACCATGGCCTGGACCCCTCTCCTGCTCCCCCTCCTCACTTTCTGCACAGTCTCTGAGGCCTCCTATGAGCTGACACAGCCACCCTCGGTGTCAGTGTCCCCAGGACAAACGGCCAGGATCACCTGCTCTGGAGATGCATTGCCAAAAAAATATGCTTATTGGTACCAGCAGAAGTCGGGCCAGGCCCCTGTGCTGGTCATCTATGAGGACAGCAAACGACCCTCCGGGATCCCTGGGAGATTCTCGGGCTCCACCTCAGGGACAATGGCCACCTTGACTATCAGTGGGGCCCAGGTGGAGGATGAAGCTGACTACTACTGTTACTCAACAGACAGCAGTACTAATTATAGGGTGTTCGGCGGAGGGACCAAGCTGACCGTCCTAGGTCAGCCCAAGGCTGCCCCCTCGGTCACTCTGTTCCCACCCTCCTCTGAGGAGCTTCAAGCCAACAAGGCCACACTGGTGTGTCTCATAAGTGACTTCTACCCGGGAGCCGTGGCAGTGGCCTGGAAGGCAGATAGCAGCCCCGTCGAGGCGGGAGTGGAGACCACCACACCCTCCAAACAAAGCAACAACAAGTACGCGGCCAGCAGCTA</t>
+  </si>
+  <si>
+    <t>96.9*</t>
   </si>
 </sst>
 </file>
@@ -472,11 +490,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,9 +512,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -535,7 +552,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -641,7 +658,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -783,7 +800,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -791,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{307334BA-5010-C54E-9B0E-47D4FB4A56AB}">
-  <dimension ref="A1:W14"/>
+  <dimension ref="A1:W15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1686,71 +1703,139 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>29729</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" t="s">
         <v>120</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" t="s">
         <v>92</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" t="s">
         <v>121</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" t="s">
         <v>23</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" t="s">
         <v>24</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" t="s">
         <v>25</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="J14" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14">
         <v>0.42255366140112499</v>
       </c>
-      <c r="L14" s="2">
-        <v>0</v>
-      </c>
-      <c r="M14" s="2">
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
         <v>1.5884815929753699</v>
       </c>
-      <c r="N14" s="2">
-        <v>0</v>
-      </c>
-      <c r="O14" s="2">
-        <v>0</v>
-      </c>
-      <c r="P14" s="2" t="s">
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14" t="s">
         <v>122</v>
       </c>
-      <c r="Q14" s="2" t="s">
+      <c r="Q14" t="s">
         <v>123</v>
       </c>
-      <c r="R14" s="2">
+      <c r="R14">
         <v>95.6</v>
       </c>
-      <c r="S14" s="3" t="s">
+      <c r="S14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="T14" s="2" t="s">
+      <c r="T14" t="s">
         <v>124</v>
       </c>
-      <c r="U14" s="3">
+      <c r="U14" s="2">
         <v>98.2</v>
       </c>
-      <c r="V14" s="3" t="s">
+      <c r="V14" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>9070</v>
+      </c>
+      <c r="B15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" t="s">
+        <v>126</v>
+      </c>
+      <c r="E15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" t="s">
+        <v>61</v>
+      </c>
+      <c r="H15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" t="s">
+        <v>72</v>
+      </c>
+      <c r="K15">
+        <v>1.27469418126954</v>
+      </c>
+      <c r="L15">
+        <v>0.47296927299907199</v>
+      </c>
+      <c r="M15">
+        <v>0.26627588651533601</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>128</v>
+      </c>
+      <c r="R15" t="s">
+        <v>130</v>
+      </c>
+      <c r="S15" t="s">
+        <v>32</v>
+      </c>
+      <c r="T15" t="s">
+        <v>129</v>
+      </c>
+      <c r="U15">
+        <v>97.6</v>
+      </c>
+      <c r="V15" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>